<commit_message>
Get V-SLAM Pose Date
</commit_message>
<xml_diff>
--- a/Doc/自定义控制协议/自主控制协议.xlsx
+++ b/Doc/自定义控制协议/自主控制协议.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23530"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\GITHUB_PROJECT\ANO_Quadcopter_2021TI\Doc\自定义控制协议\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jason\Desktop\ANO_Quadcopter_2021TI\Doc\自定义控制协议\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F7D91E2-61ED-4111-AE77-F5FA1C76E843}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F0BEA6EA-1DD3-4318-8987-C299D2E125F0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="196" uniqueCount="108">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="116">
   <si>
     <t>帧头</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -431,6 +431,38 @@
   </si>
   <si>
     <t>返回请求的色彩阈值</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>V-SLAM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>T265的位姿数据</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x轴速度 cm/s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y轴速度 cm/s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>z轴速度 cm/s</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>x轴坐标 cm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>y轴坐标 cm</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>z轴坐标 cm</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -538,7 +570,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -596,6 +628,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -884,12 +919,12 @@
       <selection activeCell="B42" sqref="B42"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="20.77734375" defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="20.75" defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="16384" width="20.77734375" style="1"/>
+    <col min="1" max="16384" width="20.75" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -912,7 +947,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:7" s="8" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A2" s="7" t="s">
         <v>7</v>
       </c>
@@ -920,13 +955,13 @@
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:7" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="5" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="5" t="s">
         <v>45</v>
       </c>
@@ -934,7 +969,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A7" s="5" t="s">
         <v>47</v>
       </c>
@@ -942,7 +977,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="5" t="s">
         <v>49</v>
       </c>
@@ -950,7 +985,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A9" s="5" t="s">
         <v>51</v>
       </c>
@@ -958,7 +993,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="5" t="s">
         <v>52</v>
       </c>
@@ -966,7 +1001,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A11" s="5" t="s">
         <v>55</v>
       </c>
@@ -974,7 +1009,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A12" s="5" t="s">
         <v>56</v>
       </c>
@@ -982,7 +1017,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A13" s="5" t="s">
         <v>57</v>
       </c>
@@ -990,7 +1025,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14" s="5" t="s">
         <v>58</v>
       </c>
@@ -998,18 +1033,18 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15" s="5" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" s="8" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="18" spans="1:14" ht="14.4" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="19" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="14.5" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="19" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
         <v>2</v>
       </c>
@@ -1050,7 +1085,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="20" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A20" s="5" t="s">
         <v>36</v>
       </c>
@@ -1081,7 +1116,7 @@
       </c>
       <c r="N20" s="16"/>
     </row>
-    <row r="21" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A21" s="5" t="s">
         <v>11</v>
       </c>
@@ -1095,7 +1130,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A22" s="5" t="s">
         <v>25</v>
       </c>
@@ -1122,42 +1157,42 @@
       </c>
       <c r="J22" s="17"/>
     </row>
-    <row r="23" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A23" s="5" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A24" s="5" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="25" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A25" s="5" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="26" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A26" s="5" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="27" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A27" s="5" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="28" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A28" s="5" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="29" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A29" s="5" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="30" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A30" s="5" t="s">
         <v>37</v>
       </c>
@@ -1174,52 +1209,52 @@
         <v>24</v>
       </c>
     </row>
-    <row r="31" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A31" s="5" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="32" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:14" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A32" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="33" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A33" s="5" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="34" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A34" s="5" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="35" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A35" s="5" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="36" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A36" s="5" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="37" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A37" s="5" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="38" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38" s="5" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="39" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39" s="5" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="40" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40" s="5" t="s">
         <v>71</v>
       </c>
@@ -1230,42 +1265,42 @@
         <v>73</v>
       </c>
     </row>
-    <row r="41" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41" s="5"/>
     </row>
-    <row r="42" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42" s="5"/>
     </row>
-    <row r="43" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43" s="5"/>
     </row>
-    <row r="44" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A44" s="5"/>
     </row>
-    <row r="45" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A45" s="5"/>
     </row>
-    <row r="46" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A46" s="5"/>
     </row>
-    <row r="47" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A47" s="5"/>
     </row>
-    <row r="48" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A48" s="5"/>
     </row>
-    <row r="49" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A49" s="5"/>
     </row>
-    <row r="50" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" s="6" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A50" s="5"/>
     </row>
-    <row r="51" spans="1:1" s="8" customFormat="1" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:1" s="8" customFormat="1" ht="14.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A51" s="7"/>
     </row>
-    <row r="52" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="53" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="54" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
+    <row r="52" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="53" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
+    <row r="54" spans="1:1" s="2" customFormat="1" x14ac:dyDescent="0.3"/>
   </sheetData>
   <mergeCells count="6">
     <mergeCell ref="M20:N20"/>
@@ -1285,17 +1320,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6EE5C0F1-A13E-4A07-9820-2FCF0A9E63D4}">
   <dimension ref="A1:P28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E12" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E26" sqref="E26:J26"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O10" sqref="O10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="8.9140625" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="30" width="30.77734375" style="13" customWidth="1"/>
-    <col min="31" max="16384" width="8.88671875" style="13"/>
+    <col min="1" max="30" width="30.75" style="13" customWidth="1"/>
+    <col min="31" max="16384" width="8.9140625" style="13"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" s="10" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="9" t="s">
         <v>2</v>
       </c>
@@ -1339,7 +1374,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A2" s="11" t="s">
         <v>36</v>
       </c>
@@ -1370,7 +1405,7 @@
       </c>
       <c r="N2" s="18"/>
     </row>
-    <row r="3" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>11</v>
       </c>
@@ -1384,7 +1419,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="4" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>25</v>
       </c>
@@ -1411,42 +1446,42 @@
       </c>
       <c r="J4" s="18"/>
     </row>
-    <row r="5" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="7" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="8" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="10" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="12" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>37</v>
       </c>
@@ -1463,47 +1498,77 @@
         <v>24</v>
       </c>
     </row>
-    <row r="13" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="14" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B13" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="E13" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="20"/>
+      <c r="G13" s="20" t="s">
+        <v>111</v>
+      </c>
+      <c r="H13" s="20"/>
+      <c r="I13" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="J13" s="20"/>
+      <c r="K13" s="20" t="s">
+        <v>113</v>
+      </c>
+      <c r="L13" s="20"/>
+      <c r="M13" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="N13" s="20"/>
+      <c r="O13" s="20" t="s">
+        <v>115</v>
+      </c>
+      <c r="P13" s="20"/>
+    </row>
+    <row r="14" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A14" s="11" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="15" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A15" s="11" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="16" spans="1:14" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A16" s="11" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="17" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="19" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="20" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="21" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>69</v>
       </c>
@@ -1511,7 +1576,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="22" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:16" s="12" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>71</v>
       </c>
@@ -1555,7 +1620,7 @@
       </c>
       <c r="P22" s="18"/>
     </row>
-    <row r="23" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A23" s="13" t="s">
         <v>88</v>
       </c>
@@ -1569,7 +1634,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="24" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="13" t="s">
         <v>93</v>
       </c>
@@ -1598,7 +1663,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="25" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A25" s="13" t="s">
         <v>94</v>
       </c>
@@ -1612,7 +1677,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="26" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A26" s="13" t="s">
         <v>95</v>
       </c>
@@ -1641,7 +1706,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="27" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="13" t="s">
         <v>96</v>
       </c>
@@ -1664,7 +1729,7 @@
       </c>
       <c r="J27" s="18"/>
     </row>
-    <row r="28" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:16" ht="30" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="13" t="s">
         <v>105</v>
       </c>
@@ -1679,7 +1744,9 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
+  <mergeCells count="18">
+    <mergeCell ref="M13:N13"/>
+    <mergeCell ref="O13:P13"/>
     <mergeCell ref="M2:N2"/>
     <mergeCell ref="K22:L22"/>
     <mergeCell ref="M22:N22"/>
@@ -1692,13 +1759,17 @@
     <mergeCell ref="G2:H2"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="K2:L2"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="G13:H13"/>
+    <mergeCell ref="I13:J13"/>
+    <mergeCell ref="K13:L13"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
     <hyperlink ref="C22" location="'0xa0'!A2" display="'0xa0'!A2" xr:uid="{9C16A3BC-2459-4D04-9BB3-51627005E9EC}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1710,14 +1781,14 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.77734375" customWidth="1"/>
-    <col min="2" max="2" width="23.77734375" customWidth="1"/>
-    <col min="3" max="23" width="20.77734375" customWidth="1"/>
+    <col min="1" max="1" width="20.75" customWidth="1"/>
+    <col min="2" max="2" width="23.75" customWidth="1"/>
+    <col min="3" max="23" width="20.75" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>83</v>
       </c>
@@ -1725,7 +1796,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>76</v>
       </c>

</xml_diff>